<commit_message>
Optimized code and Object Oriented it.
Cleaned up code
</commit_message>
<xml_diff>
--- a/Attachment 3-Attribute Names & Engineering Units.xlsx
+++ b/Attachment 3-Attribute Names & Engineering Units.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://clearwayenergy.sharepoint.com/sites/OperationsIT/Standards/Utility/EPC Exhibit A-11 Package 3.0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\A&amp;I\Projects\21431 - Mortenson CEG Solar Nova 1 &amp; 2\04 - Working Files\14 - Master IO List\Validation Folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="656" documentId="13_ncr:1_{4BD359D7-C9DB-4D4F-881C-1F9AC5E9D2AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01373C0E-C8DA-4177-AED8-5040612C0D70}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F658C621-56BF-4062-B11C-16C5CD1F22CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="728" firstSheet="3" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1290" yWindow="1380" windowWidth="21600" windowHeight="11385" tabRatio="728" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TagNaming Criteria and Examples" sheetId="12" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2084" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2138" uniqueCount="500">
   <si>
     <t>Point Names follow the naming convention:</t>
   </si>
@@ -1667,30 +1667,6 @@
     <t>Temperature-Max</t>
   </si>
   <si>
-    <t>Tracker_Commanded Tilt AngleA</t>
-  </si>
-  <si>
-    <t>Tracker_Commanded Tilt AngleB</t>
-  </si>
-  <si>
-    <t>Tracker_Commanded Tilt AngleC</t>
-  </si>
-  <si>
-    <t>Tracker_Commanded Tilt AngleD</t>
-  </si>
-  <si>
-    <t>Tracker_Commanded Tilt AngleE</t>
-  </si>
-  <si>
-    <t>Tracker_Commanded Tilt AngleF</t>
-  </si>
-  <si>
-    <t>Tracker_Commanded Tilt AngleG</t>
-  </si>
-  <si>
-    <t>Tracker_Commanded Tilt AngleH</t>
-  </si>
-  <si>
     <t>Voltage DC N</t>
   </si>
   <si>
@@ -1752,6 +1728,30 @@
   </si>
   <si>
     <t>Repeat these two lines for each motor connected to this controller</t>
+  </si>
+  <si>
+    <t>Tracker-Commanded Tilt AngleA</t>
+  </si>
+  <si>
+    <t>Tracker-Commanded Tilt AngleB</t>
+  </si>
+  <si>
+    <t>Tracker-Commanded Tilt AngleC</t>
+  </si>
+  <si>
+    <t>Tracker-Commanded Tilt AngleD</t>
+  </si>
+  <si>
+    <t>Tracker-Commanded Tilt AngleE</t>
+  </si>
+  <si>
+    <t>Tracker-Commanded Tilt AngleF</t>
+  </si>
+  <si>
+    <t>Tracker-Commanded Tilt AngleG</t>
+  </si>
+  <si>
+    <t>Tracker-Commanded Tilt AngleH</t>
   </si>
 </sst>
 </file>
@@ -1954,7 +1954,27 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="42">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -2377,7 +2397,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="DNP3.0 Points List"/>
@@ -2808,19 +2828,19 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="B17" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
       <c r="C17" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
       <c r="D17" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="E17" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -4009,7 +4029,7 @@
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="11" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -4272,7 +4292,7 @@
         <v>450</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -4291,7 +4311,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="240" verticalDpi="240" r:id="rId1"/>
@@ -4302,7 +4322,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
@@ -5166,7 +5186,7 @@
   </sheetData>
   <autoFilter ref="A1:E38" xr:uid="{270E9F6F-3E54-4333-8639-E0503346C70D}"/>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="240" verticalDpi="240" r:id="rId1"/>
@@ -5728,7 +5748,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5782,10 +5802,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="7" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5844,10 +5864,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5906,10 +5926,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5920,7 +5940,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -5928,7 +5948,7 @@
     <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="48.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5959,6 +5979,9 @@
       <c r="C2" t="s">
         <v>83</v>
       </c>
+      <c r="D2" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -5970,6 +5993,9 @@
       <c r="C3" t="s">
         <v>118</v>
       </c>
+      <c r="D3" t="s">
+        <v>432</v>
+      </c>
       <c r="E3" t="s">
         <v>433</v>
       </c>
@@ -5984,13 +6010,19 @@
       <c r="C4" t="s">
         <v>118</v>
       </c>
+      <c r="D4" t="s">
+        <v>434</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A4:A1048576 E2">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6769,16 +6801,16 @@
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="D10:D13">
-    <cfRule type="duplicateValues" dxfId="39" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10:A19 A2:A5 A7 A23:A51">
-    <cfRule type="duplicateValues" dxfId="38" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:A9">
-    <cfRule type="duplicateValues" dxfId="37" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="36" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="240" verticalDpi="240" r:id="rId1"/>
@@ -7017,31 +7049,31 @@
   </sheetData>
   <autoFilter ref="A1:B91" xr:uid="{AE146147-637B-4DFF-B80F-70F650457718}"/>
   <conditionalFormatting sqref="A16:A1048576 A1">
-    <cfRule type="duplicateValues" dxfId="35" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10:A12 A14:A15">
-    <cfRule type="duplicateValues" dxfId="34" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13">
-    <cfRule type="duplicateValues" dxfId="33" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:D12 D14:D15">
-    <cfRule type="duplicateValues" dxfId="32" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13">
-    <cfRule type="duplicateValues" dxfId="31" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A8">
-    <cfRule type="duplicateValues" dxfId="30" priority="52"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="52"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D8">
-    <cfRule type="duplicateValues" dxfId="29" priority="54"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="54"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9">
-    <cfRule type="duplicateValues" dxfId="28" priority="56"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="56"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="duplicateValues" dxfId="27" priority="58"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="58"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="240" verticalDpi="240" r:id="rId1"/>
@@ -7053,7 +7085,7 @@
   <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -8065,7 +8097,7 @@
   <autoFilter ref="A1:E69" xr:uid="{30DB61DF-688D-497A-8341-91EC4194A25F}"/>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="26" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8076,8 +8108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914127C4-5C28-4DDF-84A3-947EF29D507F}">
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -8116,6 +8148,9 @@
       <c r="C2" t="s">
         <v>118</v>
       </c>
+      <c r="D2" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -8127,6 +8162,9 @@
       <c r="C3" t="s">
         <v>118</v>
       </c>
+      <c r="D3" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -8138,6 +8176,9 @@
       <c r="C4" t="s">
         <v>118</v>
       </c>
+      <c r="D4" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -8149,6 +8190,9 @@
       <c r="C5" t="s">
         <v>118</v>
       </c>
+      <c r="D5" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -8160,6 +8204,9 @@
       <c r="C6" t="s">
         <v>118</v>
       </c>
+      <c r="D6" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -8169,6 +8216,9 @@
       <c r="C7" t="s">
         <v>118</v>
       </c>
+      <c r="D7" t="s">
+        <v>455</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -8178,6 +8228,9 @@
       <c r="C8" t="s">
         <v>118</v>
       </c>
+      <c r="D8" t="s">
+        <v>456</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -8187,6 +8240,9 @@
       <c r="C9" t="s">
         <v>118</v>
       </c>
+      <c r="D9" t="s">
+        <v>457</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -8196,6 +8252,9 @@
       <c r="C10" t="s">
         <v>118</v>
       </c>
+      <c r="D10" t="s">
+        <v>458</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -8205,6 +8264,9 @@
       <c r="C11" t="s">
         <v>118</v>
       </c>
+      <c r="D11" t="s">
+        <v>459</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -8214,6 +8276,9 @@
       <c r="C12" t="s">
         <v>118</v>
       </c>
+      <c r="D12" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -8225,6 +8290,9 @@
       <c r="C13" t="s">
         <v>118</v>
       </c>
+      <c r="D13" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -8236,6 +8304,9 @@
       <c r="C14" t="s">
         <v>118</v>
       </c>
+      <c r="D14" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -8247,6 +8318,9 @@
       <c r="C15" t="s">
         <v>118</v>
       </c>
+      <c r="D15" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -8258,8 +8332,11 @@
       <c r="C16" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>461</v>
       </c>
@@ -8269,8 +8346,11 @@
       <c r="C17" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>462</v>
       </c>
@@ -8280,8 +8360,11 @@
       <c r="C18" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>463</v>
       </c>
@@ -8291,8 +8374,11 @@
       <c r="C19" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>464</v>
       </c>
@@ -8302,8 +8388,11 @@
       <c r="C20" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>465</v>
       </c>
@@ -8313,8 +8402,11 @@
       <c r="C21" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>466</v>
       </c>
@@ -8324,8 +8416,11 @@
       <c r="C22" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>467</v>
       </c>
@@ -8335,8 +8430,11 @@
       <c r="C23" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>468</v>
       </c>
@@ -8346,8 +8444,11 @@
       <c r="C24" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>469</v>
       </c>
@@ -8357,8 +8458,11 @@
       <c r="C25" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>470</v>
       </c>
@@ -8368,10 +8472,13 @@
       <c r="C26" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>471</v>
+        <v>492</v>
       </c>
       <c r="B27" t="s">
         <v>187</v>
@@ -8379,10 +8486,13 @@
       <c r="C27" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>472</v>
+        <v>493</v>
       </c>
       <c r="B28" t="s">
         <v>187</v>
@@ -8390,10 +8500,13 @@
       <c r="C28" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>473</v>
+        <v>494</v>
       </c>
       <c r="B29" t="s">
         <v>187</v>
@@ -8401,10 +8514,13 @@
       <c r="C29" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>474</v>
+        <v>495</v>
       </c>
       <c r="B30" t="s">
         <v>187</v>
@@ -8412,10 +8528,13 @@
       <c r="C30" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>475</v>
+        <v>496</v>
       </c>
       <c r="B31" t="s">
         <v>187</v>
@@ -8423,10 +8542,13 @@
       <c r="C31" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>476</v>
+        <v>497</v>
       </c>
       <c r="B32" t="s">
         <v>187</v>
@@ -8434,10 +8556,13 @@
       <c r="C32" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>477</v>
+        <v>498</v>
       </c>
       <c r="B33" t="s">
         <v>187</v>
@@ -8445,10 +8570,13 @@
       <c r="C33" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>478</v>
+        <v>499</v>
       </c>
       <c r="B34" t="s">
         <v>187</v>
@@ -8456,8 +8584,11 @@
       <c r="C34" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>266</v>
       </c>
@@ -8467,10 +8598,13 @@
       <c r="C35" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="B36" t="s">
         <v>127</v>
@@ -8478,10 +8612,13 @@
       <c r="C36" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="B37" t="s">
         <v>127</v>
@@ -8489,10 +8626,13 @@
       <c r="C37" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="B38" t="s">
         <v>132</v>
@@ -8500,10 +8640,13 @@
       <c r="C38" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
       <c r="B39" t="s">
         <v>132</v>
@@ -8511,10 +8654,13 @@
       <c r="C39" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
       <c r="B40" t="s">
         <v>132</v>
@@ -8522,10 +8668,13 @@
       <c r="C40" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="B41" t="s">
         <v>132</v>
@@ -8533,10 +8682,13 @@
       <c r="C41" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
       <c r="B42" t="s">
         <v>132</v>
@@ -8544,10 +8696,13 @@
       <c r="C42" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
       <c r="B43" t="s">
         <v>132</v>
@@ -8555,10 +8710,13 @@
       <c r="C43" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
       <c r="B44" t="s">
         <v>132</v>
@@ -8566,10 +8724,13 @@
       <c r="C44" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="B45" t="s">
         <v>132</v>
@@ -8577,19 +8738,25 @@
       <c r="C45" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
       <c r="B46"/>
       <c r="C46" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
       <c r="B47" t="s">
         <v>230</v>
@@ -8597,19 +8764,25 @@
       <c r="C47" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
       <c r="B48"/>
       <c r="C48" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
       <c r="B49" t="s">
         <v>232</v>
@@ -8617,8 +8790,11 @@
       <c r="C49" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>254</v>
       </c>
@@ -8628,8 +8804,11 @@
       <c r="C50" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>256</v>
       </c>
@@ -8639,10 +8818,13 @@
       <c r="C51" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
       <c r="B52" t="s">
         <v>127</v>
@@ -8650,51 +8832,54 @@
       <c r="C52" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B53"/>
       <c r="C53"/>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B54"/>
       <c r="C54"/>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B55"/>
       <c r="C55"/>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B56"/>
       <c r="C56"/>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B57"/>
       <c r="C57"/>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B58"/>
       <c r="C58"/>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B59"/>
       <c r="C59"/>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B60"/>
       <c r="C60"/>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B61"/>
       <c r="C61"/>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B62"/>
       <c r="C62"/>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C63"/>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C64"/>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
@@ -8712,10 +8897,13 @@
   </sheetData>
   <autoFilter ref="A1:E64" xr:uid="{30DB61DF-688D-497A-8341-91EC4194A25F}"/>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="25" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="24" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D52">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9386,10 +9574,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A4">
-    <cfRule type="duplicateValues" dxfId="23" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="22" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="240" r:id="rId1"/>
@@ -9553,13 +9741,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A4">
-    <cfRule type="duplicateValues" dxfId="21" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="duplicateValues" dxfId="20" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="19" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10232,13 +10420,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A4 A6:A13 A17:A45">
-    <cfRule type="duplicateValues" dxfId="18" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="duplicateValues" dxfId="17" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="16" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10729,41 +10917,26 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D6:D8">
-    <cfRule type="duplicateValues" dxfId="15" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="duplicateValues" dxfId="14" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:A16 A2:A4 A6:A9 A20:A32">
-    <cfRule type="duplicateValues" dxfId="12" priority="59"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="59"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BBBB5A9BFC9FA44FAA891ECF8587AF05" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="01508630f0b5ed978d009a5c8361a6ee">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7d228c8d-f4db-4c02-93fc-107f96c3729c" xmlns:ns3="73aab363-c95c-45ea-b4e5-cbb8837b2a75" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="94dbb80d132f1caf251105561e790f47" ns2:_="" ns3:_="">
-    <xsd:import namespace="7d228c8d-f4db-4c02-93fc-107f96c3729c"/>
-    <xsd:import namespace="73aab363-c95c-45ea-b4e5-cbb8837b2a75"/>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C9FD9213F1C57D4DA5151FD7731410CA" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5bd95fbd26d2b6733914c27e62ba1a34">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4cdc74e1-130d-4383-a5f4-2197c65bc17b" xmlns:ns3="06d0c811-31c7-4f71-b442-763d52498b29" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="854f542df4a15e5fb83c870156a6c8c9" ns2:_="" ns3:_="">
+    <xsd:import namespace="4cdc74e1-130d-4383-a5f4-2197c65bc17b"/>
+    <xsd:import namespace="06d0c811-31c7-4f71-b442-763d52498b29"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -10777,8 +10950,12 @@
                 <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -10786,7 +10963,7 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="7d228c8d-f4db-4c02-93fc-107f96c3729c" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="4cdc74e1-130d-4383-a5f4-2197c65bc17b" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
@@ -10816,18 +10993,37 @@
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceAutoTags" ma:index="15" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+    <xsd:element name="MediaLengthInSeconds" ma:index="15" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="17" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="989d098c-891b-474e-9188-5175d9458c0f" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="19" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="20" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="16" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+    <xsd:element name="MediaServiceEventHashCode" ma:index="21" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
       <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
+        <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="73aab363-c95c-45ea-b4e5-cbb8837b2a75" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="06d0c811-31c7-4f71-b442-763d52498b29" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <xsd:element name="SharedWithUsers" ma:index="12" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
@@ -10855,6 +11051,17 @@
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="18" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{6257b599-3d58-4f27-95a6-9322032fd15c}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="06d0c811-31c7-4f71-b442-763d52498b29">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
@@ -10956,32 +11163,35 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D96781B-1881-445E-8910-97FFAA6E87E1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B36C8ED1-9097-42B4-96C5-752170CF076E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="06d0c811-31c7-4f71-b442-763d52498b29" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4cdc74e1-130d-4383-a5f4-2197c65bc17b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02E8DD3C-8F6C-49A1-94DE-5C4F72C46AE5}">
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABFAB71C-1C98-4760-8AE1-BCF0ACED694C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="7d228c8d-f4db-4c02-93fc-107f96c3729c"/>
-    <ds:schemaRef ds:uri="73aab363-c95c-45ea-b4e5-cbb8837b2a75"/>
+    <ds:schemaRef ds:uri="4cdc74e1-130d-4383-a5f4-2197c65bc17b"/>
+    <ds:schemaRef ds:uri="06d0c811-31c7-4f71-b442-763d52498b29"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -10990,4 +11200,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D96781B-1881-445E-8910-97FFAA6E87E1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B36C8ED1-9097-42B4-96C5-752170CF076E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="06d0c811-31c7-4f71-b442-763d52498b29"/>
+    <ds:schemaRef ds:uri="4cdc74e1-130d-4383-a5f4-2197c65bc17b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>